<commit_message>
how to run/start portainer
</commit_message>
<xml_diff>
--- a/how to send sms(demo)/bulk sms sending test.xlsx
+++ b/how to send sms(demo)/bulk sms sending test.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NADIM\Desktop\e-soft-txt-files\how to send sms(demo)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB263BF6-CABB-48DC-9833-EDC41F9B7615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E3BB7C-F9C4-4798-ABAD-61BE66D518DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,19 +69,19 @@
     <t xml:space="preserve">সিম্ফনি </t>
   </si>
   <si>
-    <t>8801859198366</t>
-  </si>
-  <si>
-    <t>8801711135082</t>
-  </si>
-  <si>
-    <t>8801911878411</t>
-  </si>
-  <si>
     <t>10 sept23 robi Long import test</t>
   </si>
   <si>
     <t>01841878414</t>
+  </si>
+  <si>
+    <t>8801761851751,SYMPHONY,"প্রিয় EO পার্টনার,আপনার DEC'23 মাসের ভ্যালু টার্গেট 590000 টাকা। সিম্ফনি মোবাইল।",9,80,FALSE,gp1,SYMPHONY,SYMPHONY Promotion</t>
+  </si>
+  <si>
+    <t>8801712049966,SYMPHONY,"প্রিয় EO পার্টনার,আপনার DEC'23 মাসের ভ্যালু টার্গেট 1500000 টাকা। সিম্ফনি মোবাইল।",9,81,FALSE,gp1,SYMPHONY,SYMPHONY Promotion</t>
+  </si>
+  <si>
+    <t>8801712288755,SYMPHONY,"প্রিয় EO পার্টনার,আপনার DEC'23 মাসের ভ্যালু টার্গেট 1500000 টাকা। সিম্ফনি মোবাইল।",9,81,FALSE,gp1,SYMPHONY,SYMPHONY Promotion</t>
   </si>
 </sst>
 </file>
@@ -403,12 +403,13 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="16.77734375" customWidth="1"/>
+    <col min="7" max="7" width="40.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -442,10 +443,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -466,15 +467,15 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -495,15 +496,15 @@
         <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -524,7 +525,7 @@
         <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>